<commit_message>
Newest vesion date 10/11/2020
</commit_message>
<xml_diff>
--- a/Docs/Câu hỏi For AIML.xlsx
+++ b/Docs/Câu hỏi For AIML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dữ liệu\Môn học\Trường\Học kỳ 7\Đồ án 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A611A0-65DA-456F-89C7-B447C36072F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DC5D50-CDA7-448E-8F55-F7B7D5796347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5760" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29340" yWindow="6090" windowWidth="18000" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="256">
   <si>
     <t>Trả lời</t>
   </si>
@@ -831,9 +831,6 @@
     <t>Các ngành học</t>
   </si>
   <si>
-    <t>Khoa, phòng ban</t>
-  </si>
-  <si>
     <t>Trường Đại học Kỹ thuật - Công nghệ Cần Thơ (CTUT - Can Tho University of Technology) là trường đại học công lập chuyên đào tạo khối ngành kỹ thuật tại Thành phố Cần Thơ. Trường trực thuộc Ủy ban Nhân dân Thành phố Cần Thơ, chịu sự giám sát về giáo dục của Bộ Giáo dục và Đào tạo.</t>
   </si>
   <si>
@@ -847,6 +844,45 @@
   </si>
   <si>
     <t>Bạn là sinh viên năm tư nếu khối lượng kiến thức tích lũy trên 100 tín chỉ.</t>
+  </si>
+  <si>
+    <t>Trường có 16 ngành học</t>
+  </si>
+  <si>
+    <t>1.Khoa học máy tính
+2.Khoa học dữ liệu 
+3.Hệ thống thông tin
+4.Công nghệ thông tin
+5.Kỹ thuật phần mềm
+6.Kỹ thuật hệ thống công nghiệp
+7.Quản lý công nghiệp
+8.Logistics và quản lý chuỗi cung ứng
+9.Quản lý xây dựng
+10.Công nghệ kỹ thuật công trình xây dựng
+11.Công nghệ kỹ thuật năng lượng
+12.Công nghệ kỹ thuật điện - điện tử
+13.Công nghệ kỹ thuật cơ điện tử
+14.Công nghệ kỹ thuật điều khiển và tự động hóa
+15.Công nghệ thực phẩm
+16.Công nghệ sinh học</t>
+  </si>
+  <si>
+    <t>Trường có 7 phòng ban</t>
+  </si>
+  <si>
+    <t>Trung tâm</t>
+  </si>
+  <si>
+    <t>Trường có 3 trung tâm</t>
+  </si>
+  <si>
+    <t>Phòng ban</t>
+  </si>
+  <si>
+    <t>Khoa</t>
+  </si>
+  <si>
+    <t>Trường có 7 khoa</t>
   </si>
 </sst>
 </file>
@@ -978,6 +1014,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -987,8 +1034,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -999,26 +1052,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1301,13 +1337,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:E137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.28515625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" style="14" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="47" customWidth="1"/>
     <col min="5" max="5" width="36.7109375" customWidth="1"/>
@@ -1315,7 +1351,7 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2"/>
@@ -1344,7 +1380,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="24">
         <v>2</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -1361,7 +1397,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="22"/>
       <c r="C6" s="5">
         <v>3</v>
@@ -1374,7 +1410,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="22"/>
       <c r="C7" s="5">
         <v>4</v>
@@ -1387,7 +1423,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="22"/>
       <c r="C8" s="5">
         <v>5</v>
@@ -1400,7 +1436,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="22"/>
       <c r="C9" s="5">
         <v>6</v>
@@ -1413,7 +1449,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="22"/>
       <c r="C10" s="5">
         <v>7</v>
@@ -1426,7 +1462,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="23"/>
       <c r="C11" s="5">
         <v>8</v>
@@ -1439,7 +1475,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+      <c r="A12" s="24">
         <v>3</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -1456,12 +1492,12 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="22"/>
-      <c r="C13" s="17">
+      <c r="C13" s="24">
         <v>10</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="27" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1469,43 +1505,43 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="22"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="22"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="16"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="27"/>
       <c r="E15" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="22"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="16"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="23"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="16"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+      <c r="A18" s="24">
         <v>4</v>
       </c>
       <c r="B18" s="21" t="s">
@@ -1518,11 +1554,11 @@
         <v>17</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="22"/>
       <c r="C19" s="3">
         <v>12</v>
@@ -1535,7 +1571,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="23"/>
       <c r="C20" s="3">
         <v>13</v>
@@ -1548,7 +1584,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
+      <c r="A21" s="24">
         <v>5</v>
       </c>
       <c r="B21" s="21" t="s">
@@ -1565,7 +1601,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="22"/>
       <c r="C22" s="3">
         <v>15</v>
@@ -1578,7 +1614,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="22"/>
       <c r="C23" s="3">
         <v>16</v>
@@ -1591,7 +1627,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="23"/>
       <c r="C24" s="3">
         <v>17</v>
@@ -1604,7 +1640,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
+      <c r="A25" s="24">
         <v>6</v>
       </c>
       <c r="B25" s="21" t="s">
@@ -1621,7 +1657,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="22"/>
       <c r="C26" s="3">
         <v>19</v>
@@ -1634,7 +1670,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="22"/>
       <c r="C27" s="3">
         <v>20</v>
@@ -1647,7 +1683,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="22"/>
       <c r="C28" s="5">
         <v>21</v>
@@ -1660,7 +1696,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="23"/>
       <c r="C29" s="5">
         <v>22</v>
@@ -1673,10 +1709,10 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="240" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
+      <c r="A30" s="18">
         <v>7</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="15" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="6">
@@ -1690,8 +1726,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="25"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="6">
         <v>24</v>
       </c>
@@ -1703,8 +1739,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="25"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="6">
         <v>25</v>
       </c>
@@ -1716,8 +1752,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="6">
         <v>26</v>
       </c>
@@ -1727,8 +1763,8 @@
       <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="25"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="6"/>
       <c r="D34" s="7" t="s">
         <v>46</v>
@@ -1738,8 +1774,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="25"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="6"/>
       <c r="D35" s="7" t="s">
         <v>48</v>
@@ -1749,8 +1785,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="25"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="6"/>
       <c r="D36" s="7" t="s">
         <v>50</v>
@@ -1760,8 +1796,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="25"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="16"/>
       <c r="C37" s="6">
         <v>27</v>
       </c>
@@ -1771,8 +1807,8 @@
       <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="25"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="6"/>
       <c r="D38" s="7" t="s">
         <v>53</v>
@@ -1782,8 +1818,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="25"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="6"/>
       <c r="D39" s="7" t="s">
         <v>55</v>
@@ -1793,8 +1829,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="25"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="6"/>
       <c r="D40" s="7" t="s">
         <v>57</v>
@@ -1804,8 +1840,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="25"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="16"/>
       <c r="C41" s="6">
         <v>28</v>
       </c>
@@ -1817,8 +1853,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="26"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="17"/>
       <c r="C42" s="6">
         <v>29</v>
       </c>
@@ -1830,10 +1866,10 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="13">
+      <c r="A43" s="18">
         <v>8</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>63</v>
       </c>
       <c r="C43" s="6">
@@ -1847,8 +1883,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="17"/>
       <c r="C44" s="6">
         <v>31</v>
       </c>
@@ -1860,10 +1896,10 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="13">
+      <c r="A45" s="18">
         <v>9</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="15" t="s">
         <v>70</v>
       </c>
       <c r="C45" s="6">
@@ -1877,8 +1913,8 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="25"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="6">
         <v>33</v>
       </c>
@@ -1890,8 +1926,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="25"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="16"/>
       <c r="C47" s="8">
         <v>34</v>
       </c>
@@ -1903,8 +1939,8 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="25"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="16"/>
       <c r="C48" s="8">
         <v>35</v>
       </c>
@@ -1916,8 +1952,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="25"/>
+      <c r="A49" s="19"/>
+      <c r="B49" s="16"/>
       <c r="C49" s="8">
         <v>36</v>
       </c>
@@ -1929,8 +1965,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="25"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="16"/>
       <c r="C50" s="8">
         <v>37</v>
       </c>
@@ -1942,8 +1978,8 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="25"/>
+      <c r="A51" s="19"/>
+      <c r="B51" s="16"/>
       <c r="C51" s="8">
         <v>38</v>
       </c>
@@ -1955,8 +1991,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="25"/>
+      <c r="A52" s="19"/>
+      <c r="B52" s="16"/>
       <c r="C52" s="8">
         <v>39</v>
       </c>
@@ -1968,8 +2004,8 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="25"/>
+      <c r="A53" s="19"/>
+      <c r="B53" s="16"/>
       <c r="C53" s="8">
         <v>40</v>
       </c>
@@ -1981,8 +2017,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="25"/>
+      <c r="A54" s="19"/>
+      <c r="B54" s="16"/>
       <c r="C54" s="8">
         <v>41</v>
       </c>
@@ -1994,8 +2030,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
-      <c r="B55" s="25"/>
+      <c r="A55" s="19"/>
+      <c r="B55" s="16"/>
       <c r="C55" s="8">
         <v>42</v>
       </c>
@@ -2007,8 +2043,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
-      <c r="B56" s="25"/>
+      <c r="A56" s="19"/>
+      <c r="B56" s="16"/>
       <c r="C56" s="8">
         <v>43</v>
       </c>
@@ -2020,8 +2056,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
-      <c r="B57" s="25"/>
+      <c r="A57" s="19"/>
+      <c r="B57" s="16"/>
       <c r="C57" s="8">
         <v>44</v>
       </c>
@@ -2033,8 +2069,8 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="25"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="16"/>
       <c r="C58" s="8">
         <v>45</v>
       </c>
@@ -2046,8 +2082,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="25"/>
+      <c r="A59" s="19"/>
+      <c r="B59" s="16"/>
       <c r="C59" s="8">
         <v>46</v>
       </c>
@@ -2059,8 +2095,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="25"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="16"/>
       <c r="C60" s="8">
         <v>47</v>
       </c>
@@ -2072,8 +2108,8 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="25"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="16"/>
       <c r="C61" s="8">
         <v>48</v>
       </c>
@@ -2085,8 +2121,8 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
-      <c r="B62" s="25"/>
+      <c r="A62" s="19"/>
+      <c r="B62" s="16"/>
       <c r="C62" s="8">
         <v>49</v>
       </c>
@@ -2098,8 +2134,8 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
-      <c r="B63" s="25"/>
+      <c r="A63" s="19"/>
+      <c r="B63" s="16"/>
       <c r="C63" s="8">
         <v>50</v>
       </c>
@@ -2111,8 +2147,8 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
-      <c r="B64" s="25"/>
+      <c r="A64" s="19"/>
+      <c r="B64" s="16"/>
       <c r="C64" s="8">
         <v>51</v>
       </c>
@@ -2124,8 +2160,8 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
-      <c r="B65" s="25"/>
+      <c r="A65" s="19"/>
+      <c r="B65" s="16"/>
       <c r="C65" s="8">
         <v>52</v>
       </c>
@@ -2137,8 +2173,8 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="25"/>
+      <c r="A66" s="19"/>
+      <c r="B66" s="16"/>
       <c r="C66" s="8">
         <v>53</v>
       </c>
@@ -2150,8 +2186,8 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
-      <c r="B67" s="26"/>
+      <c r="A67" s="20"/>
+      <c r="B67" s="17"/>
       <c r="C67" s="8">
         <v>54</v>
       </c>
@@ -2163,10 +2199,10 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="13">
+      <c r="A68" s="18">
         <v>10</v>
       </c>
-      <c r="B68" s="24" t="s">
+      <c r="B68" s="15" t="s">
         <v>132</v>
       </c>
       <c r="C68" s="8">
@@ -2180,8 +2216,8 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="25"/>
+      <c r="A69" s="19"/>
+      <c r="B69" s="16"/>
       <c r="C69" s="8">
         <v>56</v>
       </c>
@@ -2193,8 +2229,8 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="26"/>
+      <c r="A70" s="20"/>
+      <c r="B70" s="17"/>
       <c r="C70" s="8">
         <v>57</v>
       </c>
@@ -2206,10 +2242,10 @@
       </c>
     </row>
     <row r="71" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A71" s="13">
+      <c r="A71" s="18">
         <v>11</v>
       </c>
-      <c r="B71" s="24" t="s">
+      <c r="B71" s="15" t="s">
         <v>139</v>
       </c>
       <c r="C71" s="8">
@@ -2223,8 +2259,8 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
-      <c r="B72" s="25"/>
+      <c r="A72" s="19"/>
+      <c r="B72" s="16"/>
       <c r="C72" s="8">
         <v>59</v>
       </c>
@@ -2236,8 +2272,8 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
-      <c r="B73" s="26"/>
+      <c r="A73" s="20"/>
+      <c r="B73" s="17"/>
       <c r="C73" s="8">
         <v>60</v>
       </c>
@@ -2266,10 +2302,10 @@
       </c>
     </row>
     <row r="75" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="13">
+      <c r="A75" s="18">
         <v>13</v>
       </c>
-      <c r="B75" s="24" t="s">
+      <c r="B75" s="15" t="s">
         <v>150</v>
       </c>
       <c r="C75" s="8">
@@ -2283,8 +2319,8 @@
       </c>
     </row>
     <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
-      <c r="B76" s="25"/>
+      <c r="A76" s="19"/>
+      <c r="B76" s="16"/>
       <c r="C76" s="8">
         <v>63</v>
       </c>
@@ -2296,8 +2332,8 @@
       </c>
     </row>
     <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
-      <c r="B77" s="25"/>
+      <c r="A77" s="19"/>
+      <c r="B77" s="16"/>
       <c r="C77" s="8">
         <v>64</v>
       </c>
@@ -2305,12 +2341,12 @@
         <v>154</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A78" s="14"/>
-      <c r="B78" s="25"/>
+      <c r="A78" s="19"/>
+      <c r="B78" s="16"/>
       <c r="C78" s="8">
         <v>65</v>
       </c>
@@ -2318,12 +2354,12 @@
         <v>155</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
-      <c r="B79" s="26"/>
+      <c r="A79" s="20"/>
+      <c r="B79" s="17"/>
       <c r="C79" s="8">
         <v>66</v>
       </c>
@@ -2331,14 +2367,14 @@
         <v>156</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="13">
+      <c r="A80" s="18">
         <v>14</v>
       </c>
-      <c r="B80" s="24" t="s">
+      <c r="B80" s="15" t="s">
         <v>157</v>
       </c>
       <c r="C80" s="8">
@@ -2352,8 +2388,8 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
-      <c r="B81" s="25"/>
+      <c r="A81" s="19"/>
+      <c r="B81" s="16"/>
       <c r="C81" s="8">
         <v>68</v>
       </c>
@@ -2365,8 +2401,8 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
-      <c r="B82" s="25"/>
+      <c r="A82" s="19"/>
+      <c r="B82" s="16"/>
       <c r="C82" s="8">
         <v>69</v>
       </c>
@@ -2378,8 +2414,8 @@
       </c>
     </row>
     <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
-      <c r="B83" s="25"/>
+      <c r="A83" s="19"/>
+      <c r="B83" s="16"/>
       <c r="C83" s="8">
         <v>70</v>
       </c>
@@ -2391,8 +2427,8 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
-      <c r="B84" s="25"/>
+      <c r="A84" s="19"/>
+      <c r="B84" s="16"/>
       <c r="C84" s="8">
         <v>71</v>
       </c>
@@ -2404,8 +2440,8 @@
       </c>
     </row>
     <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
-      <c r="B85" s="25"/>
+      <c r="A85" s="19"/>
+      <c r="B85" s="16"/>
       <c r="C85" s="8">
         <v>72</v>
       </c>
@@ -2417,8 +2453,8 @@
       </c>
     </row>
     <row r="86" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
-      <c r="B86" s="26"/>
+      <c r="A86" s="20"/>
+      <c r="B86" s="17"/>
       <c r="C86" s="8">
         <v>73</v>
       </c>
@@ -2498,10 +2534,10 @@
       </c>
     </row>
     <row r="91" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="13">
+      <c r="A91" s="18">
         <v>19</v>
       </c>
-      <c r="B91" s="24" t="s">
+      <c r="B91" s="15" t="s">
         <v>181</v>
       </c>
       <c r="C91" s="8">
@@ -2515,8 +2551,8 @@
       </c>
     </row>
     <row r="92" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A92" s="14"/>
-      <c r="B92" s="25"/>
+      <c r="A92" s="19"/>
+      <c r="B92" s="16"/>
       <c r="C92" s="8">
         <v>79</v>
       </c>
@@ -2528,8 +2564,8 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A93" s="14"/>
-      <c r="B93" s="25"/>
+      <c r="A93" s="19"/>
+      <c r="B93" s="16"/>
       <c r="C93" s="8">
         <v>80</v>
       </c>
@@ -2541,8 +2577,8 @@
       </c>
     </row>
     <row r="94" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A94" s="15"/>
-      <c r="B94" s="26"/>
+      <c r="A94" s="20"/>
+      <c r="B94" s="17"/>
       <c r="C94" s="6">
         <v>81</v>
       </c>
@@ -2554,10 +2590,10 @@
       </c>
     </row>
     <row r="95" spans="1:5" ht="210" x14ac:dyDescent="0.25">
-      <c r="A95" s="13">
+      <c r="A95" s="18">
         <v>20</v>
       </c>
-      <c r="B95" s="24" t="s">
+      <c r="B95" s="15" t="s">
         <v>189</v>
       </c>
       <c r="C95" s="8">
@@ -2571,8 +2607,8 @@
       </c>
     </row>
     <row r="96" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
-      <c r="B96" s="25"/>
+      <c r="A96" s="19"/>
+      <c r="B96" s="16"/>
       <c r="C96" s="8">
         <v>83</v>
       </c>
@@ -2584,8 +2620,8 @@
       </c>
     </row>
     <row r="97" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A97" s="15"/>
-      <c r="B97" s="26"/>
+      <c r="A97" s="20"/>
+      <c r="B97" s="17"/>
       <c r="C97" s="8">
         <v>84</v>
       </c>
@@ -2597,10 +2633,10 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="210" x14ac:dyDescent="0.25">
-      <c r="A98" s="13">
+      <c r="A98" s="18">
         <v>21</v>
       </c>
-      <c r="B98" s="24" t="s">
+      <c r="B98" s="15" t="s">
         <v>196</v>
       </c>
       <c r="C98" s="8">
@@ -2614,8 +2650,8 @@
       </c>
     </row>
     <row r="99" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A99" s="14"/>
-      <c r="B99" s="25"/>
+      <c r="A99" s="19"/>
+      <c r="B99" s="16"/>
       <c r="C99" s="8">
         <v>86</v>
       </c>
@@ -2627,8 +2663,8 @@
       </c>
     </row>
     <row r="100" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A100" s="14"/>
-      <c r="B100" s="25"/>
+      <c r="A100" s="19"/>
+      <c r="B100" s="16"/>
       <c r="C100" s="8">
         <v>87</v>
       </c>
@@ -2640,8 +2676,8 @@
       </c>
     </row>
     <row r="101" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A101" s="14"/>
-      <c r="B101" s="25"/>
+      <c r="A101" s="19"/>
+      <c r="B101" s="16"/>
       <c r="C101" s="8">
         <v>88</v>
       </c>
@@ -2653,8 +2689,8 @@
       </c>
     </row>
     <row r="102" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="14"/>
-      <c r="B102" s="25"/>
+      <c r="A102" s="19"/>
+      <c r="B102" s="16"/>
       <c r="C102" s="8">
         <v>89</v>
       </c>
@@ -2666,8 +2702,8 @@
       </c>
     </row>
     <row r="103" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
-      <c r="B103" s="25"/>
+      <c r="A103" s="19"/>
+      <c r="B103" s="16"/>
       <c r="C103" s="8">
         <v>90</v>
       </c>
@@ -2679,8 +2715,8 @@
       </c>
     </row>
     <row r="104" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
-      <c r="B104" s="25"/>
+      <c r="A104" s="19"/>
+      <c r="B104" s="16"/>
       <c r="C104" s="8">
         <v>91</v>
       </c>
@@ -2692,8 +2728,8 @@
       </c>
     </row>
     <row r="105" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A105" s="14"/>
-      <c r="B105" s="25"/>
+      <c r="A105" s="19"/>
+      <c r="B105" s="16"/>
       <c r="C105" s="8">
         <v>92</v>
       </c>
@@ -2705,8 +2741,8 @@
       </c>
     </row>
     <row r="106" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A106" s="15"/>
-      <c r="B106" s="26"/>
+      <c r="A106" s="20"/>
+      <c r="B106" s="17"/>
       <c r="C106" s="8">
         <v>93</v>
       </c>
@@ -2718,10 +2754,10 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A107" s="13">
+      <c r="A107" s="18">
         <v>22</v>
       </c>
-      <c r="B107" s="24" t="s">
+      <c r="B107" s="15" t="s">
         <v>215</v>
       </c>
       <c r="C107" s="8">
@@ -2735,8 +2771,8 @@
       </c>
     </row>
     <row r="108" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A108" s="14"/>
-      <c r="B108" s="25"/>
+      <c r="A108" s="19"/>
+      <c r="B108" s="16"/>
       <c r="C108" s="8">
         <v>95</v>
       </c>
@@ -2748,8 +2784,8 @@
       </c>
     </row>
     <row r="109" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A109" s="14"/>
-      <c r="B109" s="25"/>
+      <c r="A109" s="19"/>
+      <c r="B109" s="16"/>
       <c r="C109" s="8">
         <v>96</v>
       </c>
@@ -2761,8 +2797,8 @@
       </c>
     </row>
     <row r="110" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A110" s="14"/>
-      <c r="B110" s="25"/>
+      <c r="A110" s="19"/>
+      <c r="B110" s="16"/>
       <c r="C110" s="8">
         <v>97</v>
       </c>
@@ -2774,8 +2810,8 @@
       </c>
     </row>
     <row r="111" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A111" s="14"/>
-      <c r="B111" s="25"/>
+      <c r="A111" s="19"/>
+      <c r="B111" s="16"/>
       <c r="C111" s="8">
         <v>98</v>
       </c>
@@ -2787,8 +2823,8 @@
       </c>
     </row>
     <row r="112" spans="1:5" ht="330" x14ac:dyDescent="0.25">
-      <c r="A112" s="14"/>
-      <c r="B112" s="25"/>
+      <c r="A112" s="19"/>
+      <c r="B112" s="16"/>
       <c r="C112" s="8">
         <v>99</v>
       </c>
@@ -2800,8 +2836,8 @@
       </c>
     </row>
     <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="14"/>
-      <c r="B113" s="25"/>
+      <c r="A113" s="19"/>
+      <c r="B113" s="16"/>
       <c r="C113" s="8">
         <v>100</v>
       </c>
@@ -2813,8 +2849,8 @@
       </c>
     </row>
     <row r="114" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A114" s="14"/>
-      <c r="B114" s="25"/>
+      <c r="A114" s="19"/>
+      <c r="B114" s="16"/>
       <c r="C114" s="8">
         <v>101</v>
       </c>
@@ -2826,8 +2862,8 @@
       </c>
     </row>
     <row r="115" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
-      <c r="B115" s="25"/>
+      <c r="A115" s="19"/>
+      <c r="B115" s="16"/>
       <c r="C115" s="8">
         <v>102</v>
       </c>
@@ -2839,8 +2875,8 @@
       </c>
     </row>
     <row r="116" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A116" s="15"/>
-      <c r="B116" s="26"/>
+      <c r="A116" s="20"/>
+      <c r="B116" s="17"/>
       <c r="C116" s="8">
         <v>103</v>
       </c>
@@ -2852,10 +2888,10 @@
       </c>
     </row>
     <row r="117" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A117" s="13">
+      <c r="A117" s="18">
         <v>23</v>
       </c>
-      <c r="B117" s="24" t="s">
+      <c r="B117" s="15" t="s">
         <v>236</v>
       </c>
       <c r="C117" s="8">
@@ -2869,8 +2905,8 @@
       </c>
     </row>
     <row r="118" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A118" s="15"/>
-      <c r="B118" s="26"/>
+      <c r="A118" s="20"/>
+      <c r="B118" s="17"/>
       <c r="C118" s="8">
         <v>105</v>
       </c>
@@ -2893,10 +2929,10 @@
       </c>
       <c r="D119" s="7"/>
       <c r="E119" s="7" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A120" s="8">
         <v>25</v>
       </c>
@@ -2906,32 +2942,56 @@
       <c r="C120" s="8">
         <v>107</v>
       </c>
-      <c r="D120" s="7"/>
-      <c r="E120" s="7"/>
+      <c r="D120" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9">
         <v>26</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="C121" s="9"/>
-      <c r="D121" s="7"/>
+        <v>253</v>
+      </c>
+      <c r="C121" s="9">
+        <v>108</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>250</v>
+      </c>
       <c r="E121" s="7"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="9"/>
-      <c r="B122" s="4"/>
-      <c r="C122" s="9"/>
-      <c r="D122" s="7"/>
+      <c r="A122" s="9">
+        <v>27</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C122" s="9">
+        <v>109</v>
+      </c>
+      <c r="D122" s="7" t="s">
+        <v>252</v>
+      </c>
       <c r="E122" s="7"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="9"/>
-      <c r="B123" s="4"/>
-      <c r="C123" s="9"/>
-      <c r="D123" s="7"/>
+      <c r="A123" s="9">
+        <v>28</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C123" s="9">
+        <v>110</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>255</v>
+      </c>
       <c r="E123" s="7"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3034,26 +3094,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="B98:B106"/>
-    <mergeCell ref="A98:A106"/>
-    <mergeCell ref="B75:B79"/>
-    <mergeCell ref="A75:A79"/>
-    <mergeCell ref="B80:B86"/>
-    <mergeCell ref="A80:A86"/>
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B30:B42"/>
-    <mergeCell ref="A30:A42"/>
     <mergeCell ref="B107:B116"/>
     <mergeCell ref="A107:A116"/>
     <mergeCell ref="B117:B118"/>
@@ -3070,6 +3110,26 @@
     <mergeCell ref="A68:A70"/>
     <mergeCell ref="B71:B73"/>
     <mergeCell ref="A71:A73"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B30:B42"/>
+    <mergeCell ref="A30:A42"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="B98:B106"/>
+    <mergeCell ref="A98:A106"/>
+    <mergeCell ref="B75:B79"/>
+    <mergeCell ref="A75:A79"/>
+    <mergeCell ref="B80:B86"/>
+    <mergeCell ref="A80:A86"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="A91:A94"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>